<commit_message>
Added comments to both MGI and Infinium templates
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Experiment_Infinium_24_v3_5_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Experiment_Infinium_24_v3_5_0.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/tests/valid_templates/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14446785-5EE6-3846-82F5-77ACB8D89B72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16360" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Experiments" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Samples" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Work" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Experiments" sheetId="1" r:id="rId1"/>
+    <sheet name="Samples" sheetId="2" r:id="rId2"/>
+    <sheet name="Work" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,12 +27,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author> </author>
+    <author/>
   </authors>
   <commentList>
-    <comment ref="B10" authorId="0">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -37,11 +42,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Infinium chip Barcode</t>
+          <t>Infinium chip Barcode</t>
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="0">
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -51,11 +56,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">provided with the kit</t>
+          <t>provided with the kit</t>
         </r>
       </text>
     </comment>
-    <comment ref="K10" authorId="0">
+    <comment ref="L10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -65,11 +70,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">date and time</t>
+          <t>date and time</t>
         </r>
       </text>
     </comment>
-    <comment ref="L10" authorId="0">
+    <comment ref="M10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -79,11 +84,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">date and time</t>
+          <t>date and time</t>
         </r>
       </text>
     </comment>
-    <comment ref="S10" authorId="0">
+    <comment ref="T10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -93,11 +98,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">until 4 barcodes per 96 well plate for 24 Sentrix format chip</t>
+          <t>until 4 barcodes per 96 well plate for 24 Sentrix format chip</t>
         </r>
       </text>
     </comment>
-    <comment ref="W10" authorId="0">
+    <comment ref="X10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -107,11 +112,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">date and time</t>
+          <t>date and time</t>
         </r>
       </text>
     </comment>
-    <comment ref="X10" authorId="0">
+    <comment ref="Y10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -121,11 +126,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">date and time</t>
+          <t>date and time</t>
         </r>
       </text>
     </comment>
-    <comment ref="AM10" authorId="0">
+    <comment ref="AN10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -135,11 +140,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">This field is present only for lab validation. It will not be stored. It should match Experiment Container Barcode.</t>
+          <t>This field is present only for lab validation. It will not be stored. It should match Experiment Container Barcode.</t>
         </r>
       </text>
     </comment>
-    <comment ref="AN10" authorId="0">
+    <comment ref="AO10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -149,7 +154,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">can handle 4 chip max</t>
+          <t>can handle 4 chip max</t>
         </r>
       </text>
     </comment>
@@ -158,345 +163,346 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="109">
-  <si>
-    <t xml:space="preserve">Experiment Submission Template</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Run Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Infinium Global Screening Array-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Template Version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fill the Experiments page with the information common to all samples in each experiment, then detail information specific to each sample on the Samples page.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If a sample appears in more than one experiment, enter multiple entries with the information pertaining to each experiment with the appropriate experiment ID.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Experiment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amplification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fragmentation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Precipitation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hybridization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wash beadchip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extend and Stain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Image (scan)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Experiment Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Experiment Container Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Experiment Container Kind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instrument Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Experiment Start Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSA3 Plate Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1N NaOH formulation date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reagent MA1 Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reagent MA2 Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reagent MSM Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incubation time In Amplification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incubation time Out Amplification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comment Amplification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reagent FMS Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comment Fragmentation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reagent PM1 Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reagent RA1 Barcode Precipitation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comment Precipitation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hybridization Chip Barcodes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hybridization Chamber Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reagent PB2 Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reagent XC4 Barcode Hybridization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incubation time In Hybridization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incubation time Out Hybridization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comment Hybridization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reagent PB1 Barcode Wash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comment Wash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">95% form/EDTA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reagent ATM Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reagent EML Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reagent LX1 Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reagent LX2 Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reagent PB1 Barcode Stain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reagent RA1 Barcode Stain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reagent SML Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reagent XC3 Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reagent XC4 Barcode Stain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comment Stain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SentrixBarcode_A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scan Chip Rack Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comment Scan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TestExp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">infinium gs 24 beadchip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">iScan_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PlateBarcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ReagentAmpBarcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ReagentMA2BarcodeHere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSMBarcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FragFMSBarcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">short comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pm1Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ra1PrecipBarcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HybrBarcodeValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HCBarcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PB2Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XC4HyBarcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">my comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">washbeadchipbarcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">atmbarcodehere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testbarcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lx1barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lx2barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pb1stain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ra1stain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">smltest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xc3value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xc4stain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sentrixA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lastbarcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bla bla bla</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample Preparation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source Container Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source Container Coordinates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source Sample Volume Used</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Experiment Container Coordinates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EQ00539851</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fragment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Precipitate and Resuspend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hybridize</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wash BeadChip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Image (Scan)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSA3 Plate Barcode (provides with the kit)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chip Barcodes (until 4 barcodes per 96 well plate for 24 Sentrix format chip)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reagent PB1 Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chip Barcode (until 4 barcodes per 96 well plate for 24 Sentrix format chip)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reagent RA1 Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chip Rack Barcode (can handle 4 chip max)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reagent XC4 Barcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incubation time In (date and time)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incubation time Out (date and time)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="110">
+  <si>
+    <t>Experiment Submission Template</t>
+  </si>
+  <si>
+    <t>Run Type</t>
+  </si>
+  <si>
+    <t>Infinium Global Screening Array-24</t>
+  </si>
+  <si>
+    <t>Template Version</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Fill the Experiments page with the information common to all samples in each experiment, then detail information specific to each sample on the Samples page.</t>
+  </si>
+  <si>
+    <t>If a sample appears in more than one experiment, enter multiple entries with the information pertaining to each experiment with the appropriate experiment ID.</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+  </si>
+  <si>
+    <t>Amplification</t>
+  </si>
+  <si>
+    <t>Fragmentation</t>
+  </si>
+  <si>
+    <t>Precipitation</t>
+  </si>
+  <si>
+    <t>Hybridization</t>
+  </si>
+  <si>
+    <t>Wash beadchip</t>
+  </si>
+  <si>
+    <t>Extend and Stain</t>
+  </si>
+  <si>
+    <t>Image (scan)</t>
+  </si>
+  <si>
+    <t>Experiment Name</t>
+  </si>
+  <si>
+    <t>Experiment Container Barcode</t>
+  </si>
+  <si>
+    <t>Experiment Container Kind</t>
+  </si>
+  <si>
+    <t>Instrument Name</t>
+  </si>
+  <si>
+    <t>Experiment Start Date</t>
+  </si>
+  <si>
+    <t>MSA3 Plate Barcode</t>
+  </si>
+  <si>
+    <t>0.1N NaOH formulation date</t>
+  </si>
+  <si>
+    <t>Reagent MA1 Barcode</t>
+  </si>
+  <si>
+    <t>Reagent MA2 Barcode</t>
+  </si>
+  <si>
+    <t>Reagent MSM Barcode</t>
+  </si>
+  <si>
+    <t>Incubation time In Amplification</t>
+  </si>
+  <si>
+    <t>Incubation time Out Amplification</t>
+  </si>
+  <si>
+    <t>Comment Amplification</t>
+  </si>
+  <si>
+    <t>Reagent FMS Barcode</t>
+  </si>
+  <si>
+    <t>Comment Fragmentation</t>
+  </si>
+  <si>
+    <t>Reagent PM1 Barcode</t>
+  </si>
+  <si>
+    <t>Reagent RA1 Barcode Precipitation</t>
+  </si>
+  <si>
+    <t>Comment Precipitation</t>
+  </si>
+  <si>
+    <t>Hybridization Chip Barcodes</t>
+  </si>
+  <si>
+    <t>Hybridization Chamber Barcode</t>
+  </si>
+  <si>
+    <t>Reagent PB2 Barcode</t>
+  </si>
+  <si>
+    <t>Reagent XC4 Barcode Hybridization</t>
+  </si>
+  <si>
+    <t>Incubation time In Hybridization</t>
+  </si>
+  <si>
+    <t>Incubation time Out Hybridization</t>
+  </si>
+  <si>
+    <t>Comment Hybridization</t>
+  </si>
+  <si>
+    <t>Reagent PB1 Barcode Wash</t>
+  </si>
+  <si>
+    <t>Comment Wash</t>
+  </si>
+  <si>
+    <t>95% form/EDTA</t>
+  </si>
+  <si>
+    <t>Reagent ATM Barcode</t>
+  </si>
+  <si>
+    <t>Reagent EML Barcode</t>
+  </si>
+  <si>
+    <t>Reagent LX1 Barcode</t>
+  </si>
+  <si>
+    <t>Reagent LX2 Barcode</t>
+  </si>
+  <si>
+    <t>Reagent PB1 Barcode Stain</t>
+  </si>
+  <si>
+    <t>Reagent RA1 Barcode Stain</t>
+  </si>
+  <si>
+    <t>Reagent SML Barcode</t>
+  </si>
+  <si>
+    <t>Reagent XC3 Barcode</t>
+  </si>
+  <si>
+    <t>Reagent XC4 Barcode Stain</t>
+  </si>
+  <si>
+    <t>Comment Stain</t>
+  </si>
+  <si>
+    <t>SentrixBarcode_A</t>
+  </si>
+  <si>
+    <t>Scan Chip Rack Barcode</t>
+  </si>
+  <si>
+    <t>Comment Scan</t>
+  </si>
+  <si>
+    <t>TestExp</t>
+  </si>
+  <si>
+    <t>hh</t>
+  </si>
+  <si>
+    <t>infinium gs 24 beadchip</t>
+  </si>
+  <si>
+    <t>iScan_1</t>
+  </si>
+  <si>
+    <t>PlateBarcode</t>
+  </si>
+  <si>
+    <t>ReagentAmpBarcode</t>
+  </si>
+  <si>
+    <t>ReagentMA2BarcodeHere</t>
+  </si>
+  <si>
+    <t>MSMBarcode</t>
+  </si>
+  <si>
+    <t>FragFMSBarcode</t>
+  </si>
+  <si>
+    <t>short comment</t>
+  </si>
+  <si>
+    <t>Pm1Barcode</t>
+  </si>
+  <si>
+    <t>Ra1PrecipBarcode</t>
+  </si>
+  <si>
+    <t>HybrBarcodeValue</t>
+  </si>
+  <si>
+    <t>HCBarcode</t>
+  </si>
+  <si>
+    <t>PB2Barcode</t>
+  </si>
+  <si>
+    <t>XC4HyBarcode</t>
+  </si>
+  <si>
+    <t>my comment</t>
+  </si>
+  <si>
+    <t>washbeadchipbarcode</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>atmbarcodehere</t>
+  </si>
+  <si>
+    <t>testbarcode</t>
+  </si>
+  <si>
+    <t>lx1barcode</t>
+  </si>
+  <si>
+    <t>lx2barcode</t>
+  </si>
+  <si>
+    <t>pb1stain</t>
+  </si>
+  <si>
+    <t>ra1stain</t>
+  </si>
+  <si>
+    <t>smltest</t>
+  </si>
+  <si>
+    <t>xc3value</t>
+  </si>
+  <si>
+    <t>xc4stain</t>
+  </si>
+  <si>
+    <t>sentrixA</t>
+  </si>
+  <si>
+    <t>lastbarcode</t>
+  </si>
+  <si>
+    <t>bla bla bla</t>
+  </si>
+  <si>
+    <t>Sample Preparation</t>
+  </si>
+  <si>
+    <t>Source Container Barcode</t>
+  </si>
+  <si>
+    <t>Source Container Coordinates</t>
+  </si>
+  <si>
+    <t>Source Sample Volume Used</t>
+  </si>
+  <si>
+    <t>Experiment Container Coordinates</t>
+  </si>
+  <si>
+    <t>EQ00539851</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>Fragment</t>
+  </si>
+  <si>
+    <t>Precipitate and Resuspend</t>
+  </si>
+  <si>
+    <t>Hybridize</t>
+  </si>
+  <si>
+    <t>Wash BeadChip</t>
+  </si>
+  <si>
+    <t>Image (Scan)</t>
+  </si>
+  <si>
+    <t>MSA3 Plate Barcode (provides with the kit)</t>
+  </si>
+  <si>
+    <t>Chip Barcodes (until 4 barcodes per 96 well plate for 24 Sentrix format chip)</t>
+  </si>
+  <si>
+    <t>Reagent PB1 Barcode</t>
+  </si>
+  <si>
+    <t>Chip Barcode (until 4 barcodes per 96 well plate for 24 Sentrix format chip)</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Reagent RA1 Barcode</t>
+  </si>
+  <si>
+    <t>Chip Rack Barcode (can handle 4 chip max)</t>
+  </si>
+  <si>
+    <t>Reagent XC4 Barcode</t>
+  </si>
+  <si>
+    <t>Incubation time In (date and time)</t>
+  </si>
+  <si>
+    <t>Incubation time Out (date and time)</t>
+  </si>
+  <si>
+    <t>Test comment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="166" formatCode="h:mm"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -505,22 +511,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -611,213 +602,131 @@
     </fill>
   </fills>
   <borders count="5">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="hair"/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="dashed"/>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
-      <right style="dashed"/>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="35">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="34">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -876,79 +785,386 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF1F497D"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AMI106"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMJ106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="24.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="27.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="28.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="19.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="23.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="26.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="19.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="22.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="13.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="19.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="20.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="31" style="0" width="20.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="23.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="22.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="18.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="18.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="22.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="13.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="39" style="0" width="25.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="15.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1019" style="0" width="9.17"/>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="2" max="2" width="48.5" customWidth="1"/>
+    <col min="3" max="3" width="37.83203125" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" customWidth="1"/>
+    <col min="5" max="6" width="24.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.83203125" customWidth="1"/>
+    <col min="8" max="8" width="27.5" customWidth="1"/>
+    <col min="9" max="10" width="21.1640625" customWidth="1"/>
+    <col min="11" max="11" width="21.83203125" customWidth="1"/>
+    <col min="12" max="12" width="26.6640625" customWidth="1"/>
+    <col min="13" max="13" width="27.83203125" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" customWidth="1"/>
+    <col min="15" max="15" width="21" customWidth="1"/>
+    <col min="16" max="16" width="20.83203125" customWidth="1"/>
+    <col min="17" max="17" width="21" customWidth="1"/>
+    <col min="18" max="18" width="28.83203125" customWidth="1"/>
+    <col min="19" max="19" width="19.1640625" customWidth="1"/>
+    <col min="20" max="20" width="23.1640625" customWidth="1"/>
+    <col min="21" max="21" width="26.1640625" customWidth="1"/>
+    <col min="22" max="22" width="20.5" customWidth="1"/>
+    <col min="23" max="23" width="32" customWidth="1"/>
+    <col min="24" max="24" width="26.6640625" customWidth="1"/>
+    <col min="25" max="25" width="35" customWidth="1"/>
+    <col min="26" max="26" width="19.6640625" customWidth="1"/>
+    <col min="27" max="27" width="22.83203125" customWidth="1"/>
+    <col min="28" max="28" width="13.6640625" customWidth="1"/>
+    <col min="29" max="29" width="19.1640625" customWidth="1"/>
+    <col min="30" max="30" width="21.1640625" customWidth="1"/>
+    <col min="31" max="31" width="20.83203125" customWidth="1"/>
+    <col min="32" max="33" width="20.1640625" customWidth="1"/>
+    <col min="34" max="34" width="23.5" customWidth="1"/>
+    <col min="35" max="35" width="22.83203125" customWidth="1"/>
+    <col min="36" max="36" width="18.5" customWidth="1"/>
+    <col min="37" max="37" width="18.1640625" customWidth="1"/>
+    <col min="38" max="38" width="22.6640625" customWidth="1"/>
+    <col min="39" max="39" width="13.5" customWidth="1"/>
+    <col min="40" max="41" width="25.5" customWidth="1"/>
+    <col min="42" max="42" width="15.1640625" customWidth="1"/>
+    <col min="1020" max="1024" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="5"/>
-    </row>
-    <row r="3" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:1024" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -957,8 +1173,9 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="7"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
@@ -968,21 +1185,22 @@
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="9"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="F4" s="9"/>
+    </row>
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>7</v>
       </c>
@@ -990,42 +1208,42 @@
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="12"/>
+      <c r="G9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
       <c r="M9" s="14"/>
-      <c r="N9" s="15" t="s">
+      <c r="N9" s="14"/>
+      <c r="O9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="15"/>
-      <c r="P9" s="16" t="s">
+      <c r="P9" s="15"/>
+      <c r="Q9" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="Q9" s="16"/>
       <c r="R9" s="16"/>
-      <c r="S9" s="17" t="s">
+      <c r="S9" s="16"/>
+      <c r="T9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="T9" s="17"/>
       <c r="U9" s="17"/>
       <c r="V9" s="17"/>
       <c r="W9" s="17"/>
       <c r="X9" s="17"/>
       <c r="Y9" s="17"/>
-      <c r="Z9" s="18" t="s">
+      <c r="Z9" s="17"/>
+      <c r="AA9" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="AA9" s="18"/>
-      <c r="AB9" s="19" t="s">
+      <c r="AB9" s="18"/>
+      <c r="AC9" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="AC9" s="19"/>
       <c r="AD9" s="19"/>
       <c r="AE9" s="19"/>
       <c r="AF9" s="19"/>
@@ -1035,13 +1253,14 @@
       <c r="AJ9" s="19"/>
       <c r="AK9" s="19"/>
       <c r="AL9" s="19"/>
-      <c r="AM9" s="20" t="s">
+      <c r="AM9" s="19"/>
+      <c r="AN9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="AN9" s="20"/>
       <c r="AO9" s="20"/>
-    </row>
-    <row r="10" s="23" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP9" s="20"/>
+    </row>
+    <row r="10" spans="1:1024" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
         <v>15</v>
       </c>
@@ -1057,240 +1276,246 @@
       <c r="E10" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="H10" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="I10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="J10" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="K10" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="21" t="s">
+      <c r="L10" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="21" t="s">
+      <c r="M10" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="M10" s="21" t="s">
+      <c r="N10" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="N10" s="21" t="s">
+      <c r="O10" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="O10" s="21" t="s">
+      <c r="P10" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="P10" s="21" t="s">
+      <c r="Q10" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="Q10" s="21" t="s">
+      <c r="R10" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="R10" s="21" t="s">
+      <c r="S10" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="S10" s="21" t="s">
+      <c r="T10" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="T10" s="21" t="s">
+      <c r="U10" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="U10" s="21" t="s">
+      <c r="V10" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="V10" s="21" t="s">
+      <c r="W10" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="W10" s="21" t="s">
+      <c r="X10" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="X10" s="21" t="s">
+      <c r="Y10" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="Y10" s="21" t="s">
+      <c r="Z10" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="Z10" s="21" t="s">
+      <c r="AA10" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="AA10" s="21" t="s">
+      <c r="AB10" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="AB10" s="21" t="s">
+      <c r="AC10" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="AC10" s="21" t="s">
+      <c r="AD10" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="AD10" s="21" t="s">
+      <c r="AE10" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="AE10" s="21" t="s">
+      <c r="AF10" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="AF10" s="21" t="s">
+      <c r="AG10" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="AG10" s="21" t="s">
+      <c r="AH10" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="AH10" s="21" t="s">
+      <c r="AI10" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="AI10" s="21" t="s">
+      <c r="AJ10" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="AJ10" s="21" t="s">
+      <c r="AK10" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="AK10" s="21" t="s">
+      <c r="AL10" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="AL10" s="21" t="s">
+      <c r="AM10" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="AM10" s="21" t="s">
+      <c r="AN10" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="AN10" s="21" t="s">
+      <c r="AO10" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="AO10" s="21" t="s">
+      <c r="AP10" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="AME10" s="21"/>
       <c r="AMF10" s="21"/>
       <c r="AMG10" s="21"/>
       <c r="AMH10" s="21"/>
       <c r="AMI10" s="21"/>
-    </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMJ10" s="21"/>
+    </row>
+    <row r="11" spans="1:1024" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="25" t="n">
+      <c r="E11" s="25">
         <v>44198</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="G11" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="G11" s="1" t="n">
+      <c r="H11" s="1">
         <v>44289</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="I11" t="s">
         <v>61</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="J11" t="s">
         <v>62</v>
       </c>
-      <c r="J11" s="0" t="s">
+      <c r="K11" t="s">
         <v>63</v>
       </c>
-      <c r="K11" s="27" t="n">
+      <c r="L11" s="27">
         <v>0.125</v>
       </c>
-      <c r="L11" s="27" t="n">
-        <v>0.166666666666667</v>
-      </c>
-      <c r="N11" s="24" t="s">
+      <c r="M11" s="27">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="O11" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="O11" s="0" t="s">
+      <c r="P11" t="s">
         <v>65</v>
       </c>
-      <c r="P11" s="24" t="s">
+      <c r="Q11" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="Q11" s="0" t="s">
+      <c r="R11" t="s">
         <v>67</v>
       </c>
-      <c r="S11" s="24" t="s">
+      <c r="T11" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="T11" s="0" t="s">
+      <c r="U11" t="s">
         <v>69</v>
       </c>
-      <c r="U11" s="0" t="s">
+      <c r="V11" t="s">
         <v>70</v>
       </c>
-      <c r="V11" s="0" t="s">
+      <c r="W11" t="s">
         <v>71</v>
       </c>
-      <c r="W11" s="27" t="n">
-        <v>0.0833333333333333</v>
-      </c>
-      <c r="X11" s="27" t="n">
-        <v>0.0972222222222222</v>
-      </c>
-      <c r="Y11" s="0" t="s">
+      <c r="X11" s="27">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="Y11" s="27">
+        <v>9.7222222222222196E-2</v>
+      </c>
+      <c r="Z11" t="s">
         <v>72</v>
       </c>
-      <c r="Z11" s="24" t="s">
+      <c r="AA11" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="AB11" s="24" t="s">
+      <c r="AC11" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="AC11" s="0" t="s">
+      <c r="AD11" t="s">
         <v>75</v>
       </c>
-      <c r="AD11" s="0" t="s">
+      <c r="AE11" t="s">
         <v>76</v>
       </c>
-      <c r="AE11" s="0" t="s">
+      <c r="AF11" t="s">
         <v>77</v>
       </c>
-      <c r="AF11" s="0" t="s">
+      <c r="AG11" t="s">
         <v>78</v>
       </c>
-      <c r="AG11" s="0" t="s">
+      <c r="AH11" t="s">
         <v>79</v>
       </c>
-      <c r="AH11" s="0" t="s">
+      <c r="AI11" t="s">
         <v>80</v>
       </c>
-      <c r="AI11" s="0" t="s">
+      <c r="AJ11" t="s">
         <v>81</v>
       </c>
-      <c r="AJ11" s="0" t="s">
+      <c r="AK11" t="s">
         <v>82</v>
       </c>
-      <c r="AK11" s="0" t="s">
+      <c r="AL11" t="s">
         <v>83</v>
       </c>
-      <c r="AM11" s="24" t="s">
+      <c r="AN11" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="AN11" s="0" t="s">
+      <c r="AO11" t="s">
         <v>85</v>
       </c>
-      <c r="AO11" s="28" t="s">
+      <c r="AP11" s="28" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="29"/>
-      <c r="F12" s="10"/>
+      <c r="F12" s="29"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
@@ -1326,14 +1551,15 @@
       <c r="AM12" s="10"/>
       <c r="AN12" s="10"/>
       <c r="AO12" s="10"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP12" s="10"/>
+    </row>
+    <row r="13" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="29"/>
-      <c r="F13" s="10"/>
+      <c r="F13" s="29"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
@@ -1369,14 +1595,15 @@
       <c r="AM13" s="10"/>
       <c r="AN13" s="10"/>
       <c r="AO13" s="10"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP13" s="10"/>
+    </row>
+    <row r="14" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="29"/>
-      <c r="F14" s="10"/>
+      <c r="F14" s="29"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
@@ -1412,14 +1639,15 @@
       <c r="AM14" s="10"/>
       <c r="AN14" s="10"/>
       <c r="AO14" s="10"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP14" s="10"/>
+    </row>
+    <row r="15" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="29"/>
-      <c r="F15" s="10"/>
+      <c r="F15" s="29"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
@@ -1455,14 +1683,15 @@
       <c r="AM15" s="10"/>
       <c r="AN15" s="10"/>
       <c r="AO15" s="10"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP15" s="10"/>
+    </row>
+    <row r="16" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="29"/>
-      <c r="F16" s="10"/>
+      <c r="F16" s="29"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
@@ -1498,14 +1727,15 @@
       <c r="AM16" s="10"/>
       <c r="AN16" s="10"/>
       <c r="AO16" s="10"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP16" s="10"/>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="29"/>
-      <c r="F17" s="10"/>
+      <c r="F17" s="29"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
@@ -1541,14 +1771,15 @@
       <c r="AM17" s="10"/>
       <c r="AN17" s="10"/>
       <c r="AO17" s="10"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP17" s="10"/>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="29"/>
-      <c r="F18" s="10"/>
+      <c r="F18" s="29"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
@@ -1584,14 +1815,15 @@
       <c r="AM18" s="10"/>
       <c r="AN18" s="10"/>
       <c r="AO18" s="10"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP18" s="10"/>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="29"/>
-      <c r="F19" s="10"/>
+      <c r="F19" s="29"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
@@ -1627,14 +1859,15 @@
       <c r="AM19" s="10"/>
       <c r="AN19" s="10"/>
       <c r="AO19" s="10"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP19" s="10"/>
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="29"/>
-      <c r="F20" s="10"/>
+      <c r="F20" s="29"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
@@ -1670,14 +1903,15 @@
       <c r="AM20" s="10"/>
       <c r="AN20" s="10"/>
       <c r="AO20" s="10"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP20" s="10"/>
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="29"/>
-      <c r="F21" s="10"/>
+      <c r="F21" s="29"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
@@ -1713,14 +1947,15 @@
       <c r="AM21" s="10"/>
       <c r="AN21" s="10"/>
       <c r="AO21" s="10"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP21" s="10"/>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="29"/>
-      <c r="F22" s="10"/>
+      <c r="F22" s="29"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
@@ -1756,14 +1991,15 @@
       <c r="AM22" s="10"/>
       <c r="AN22" s="10"/>
       <c r="AO22" s="10"/>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP22" s="10"/>
+    </row>
+    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="29"/>
-      <c r="F23" s="10"/>
+      <c r="F23" s="29"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
@@ -1799,14 +2035,15 @@
       <c r="AM23" s="10"/>
       <c r="AN23" s="10"/>
       <c r="AO23" s="10"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP23" s="10"/>
+    </row>
+    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="29"/>
-      <c r="F24" s="10"/>
+      <c r="F24" s="29"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
@@ -1842,14 +2079,15 @@
       <c r="AM24" s="10"/>
       <c r="AN24" s="10"/>
       <c r="AO24" s="10"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP24" s="10"/>
+    </row>
+    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="29"/>
-      <c r="F25" s="10"/>
+      <c r="F25" s="29"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
@@ -1885,14 +2123,15 @@
       <c r="AM25" s="10"/>
       <c r="AN25" s="10"/>
       <c r="AO25" s="10"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP25" s="10"/>
+    </row>
+    <row r="26" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="29"/>
-      <c r="F26" s="10"/>
+      <c r="F26" s="29"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
@@ -1928,14 +2167,15 @@
       <c r="AM26" s="10"/>
       <c r="AN26" s="10"/>
       <c r="AO26" s="10"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP26" s="10"/>
+    </row>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="29"/>
-      <c r="F27" s="10"/>
+      <c r="F27" s="29"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
@@ -1971,14 +2211,15 @@
       <c r="AM27" s="10"/>
       <c r="AN27" s="10"/>
       <c r="AO27" s="10"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP27" s="10"/>
+    </row>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="29"/>
-      <c r="F28" s="10"/>
+      <c r="F28" s="29"/>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
@@ -2014,14 +2255,15 @@
       <c r="AM28" s="10"/>
       <c r="AN28" s="10"/>
       <c r="AO28" s="10"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP28" s="10"/>
+    </row>
+    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="29"/>
-      <c r="F29" s="10"/>
+      <c r="F29" s="29"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
@@ -2057,14 +2299,15 @@
       <c r="AM29" s="10"/>
       <c r="AN29" s="10"/>
       <c r="AO29" s="10"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP29" s="10"/>
+    </row>
+    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30" s="29"/>
-      <c r="F30" s="10"/>
+      <c r="F30" s="29"/>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
@@ -2100,14 +2343,15 @@
       <c r="AM30" s="10"/>
       <c r="AN30" s="10"/>
       <c r="AO30" s="10"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP30" s="10"/>
+    </row>
+    <row r="31" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A31" s="10"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
       <c r="E31" s="29"/>
-      <c r="F31" s="10"/>
+      <c r="F31" s="29"/>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
@@ -2143,14 +2387,15 @@
       <c r="AM31" s="10"/>
       <c r="AN31" s="10"/>
       <c r="AO31" s="10"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP31" s="10"/>
+    </row>
+    <row r="32" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
       <c r="E32" s="29"/>
-      <c r="F32" s="10"/>
+      <c r="F32" s="29"/>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
@@ -2186,14 +2431,15 @@
       <c r="AM32" s="10"/>
       <c r="AN32" s="10"/>
       <c r="AO32" s="10"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP32" s="10"/>
+    </row>
+    <row r="33" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
       <c r="E33" s="29"/>
-      <c r="F33" s="10"/>
+      <c r="F33" s="29"/>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
@@ -2229,14 +2475,15 @@
       <c r="AM33" s="10"/>
       <c r="AN33" s="10"/>
       <c r="AO33" s="10"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP33" s="10"/>
+    </row>
+    <row r="34" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A34" s="10"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
       <c r="E34" s="29"/>
-      <c r="F34" s="10"/>
+      <c r="F34" s="29"/>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
       <c r="I34" s="10"/>
@@ -2272,14 +2519,15 @@
       <c r="AM34" s="10"/>
       <c r="AN34" s="10"/>
       <c r="AO34" s="10"/>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP34" s="10"/>
+    </row>
+    <row r="35" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
       <c r="E35" s="29"/>
-      <c r="F35" s="10"/>
+      <c r="F35" s="29"/>
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
@@ -2315,14 +2563,15 @@
       <c r="AM35" s="10"/>
       <c r="AN35" s="10"/>
       <c r="AO35" s="10"/>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP35" s="10"/>
+    </row>
+    <row r="36" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
       <c r="E36" s="29"/>
-      <c r="F36" s="10"/>
+      <c r="F36" s="29"/>
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
       <c r="I36" s="10"/>
@@ -2358,14 +2607,15 @@
       <c r="AM36" s="10"/>
       <c r="AN36" s="10"/>
       <c r="AO36" s="10"/>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP36" s="10"/>
+    </row>
+    <row r="37" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="29"/>
-      <c r="F37" s="10"/>
+      <c r="F37" s="29"/>
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
@@ -2401,14 +2651,15 @@
       <c r="AM37" s="10"/>
       <c r="AN37" s="10"/>
       <c r="AO37" s="10"/>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP37" s="10"/>
+    </row>
+    <row r="38" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
       <c r="E38" s="29"/>
-      <c r="F38" s="10"/>
+      <c r="F38" s="29"/>
       <c r="G38" s="10"/>
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
@@ -2444,14 +2695,15 @@
       <c r="AM38" s="10"/>
       <c r="AN38" s="10"/>
       <c r="AO38" s="10"/>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP38" s="10"/>
+    </row>
+    <row r="39" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
       <c r="E39" s="29"/>
-      <c r="F39" s="10"/>
+      <c r="F39" s="29"/>
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
@@ -2487,14 +2739,15 @@
       <c r="AM39" s="10"/>
       <c r="AN39" s="10"/>
       <c r="AO39" s="10"/>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP39" s="10"/>
+    </row>
+    <row r="40" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
       <c r="E40" s="29"/>
-      <c r="F40" s="10"/>
+      <c r="F40" s="29"/>
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
@@ -2530,14 +2783,15 @@
       <c r="AM40" s="10"/>
       <c r="AN40" s="10"/>
       <c r="AO40" s="10"/>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP40" s="10"/>
+    </row>
+    <row r="41" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
       <c r="E41" s="29"/>
-      <c r="F41" s="10"/>
+      <c r="F41" s="29"/>
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
       <c r="I41" s="10"/>
@@ -2573,14 +2827,15 @@
       <c r="AM41" s="10"/>
       <c r="AN41" s="10"/>
       <c r="AO41" s="10"/>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP41" s="10"/>
+    </row>
+    <row r="42" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A42" s="10"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
       <c r="E42" s="29"/>
-      <c r="F42" s="10"/>
+      <c r="F42" s="29"/>
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
@@ -2616,14 +2871,15 @@
       <c r="AM42" s="10"/>
       <c r="AN42" s="10"/>
       <c r="AO42" s="10"/>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP42" s="10"/>
+    </row>
+    <row r="43" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A43" s="10"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
       <c r="E43" s="29"/>
-      <c r="F43" s="10"/>
+      <c r="F43" s="29"/>
       <c r="G43" s="10"/>
       <c r="H43" s="10"/>
       <c r="I43" s="10"/>
@@ -2659,14 +2915,15 @@
       <c r="AM43" s="10"/>
       <c r="AN43" s="10"/>
       <c r="AO43" s="10"/>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP43" s="10"/>
+    </row>
+    <row r="44" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A44" s="10"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
       <c r="E44" s="29"/>
-      <c r="F44" s="10"/>
+      <c r="F44" s="29"/>
       <c r="G44" s="10"/>
       <c r="H44" s="10"/>
       <c r="I44" s="10"/>
@@ -2702,14 +2959,15 @@
       <c r="AM44" s="10"/>
       <c r="AN44" s="10"/>
       <c r="AO44" s="10"/>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP44" s="10"/>
+    </row>
+    <row r="45" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A45" s="10"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
       <c r="E45" s="29"/>
-      <c r="F45" s="10"/>
+      <c r="F45" s="29"/>
       <c r="G45" s="10"/>
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
@@ -2745,14 +3003,15 @@
       <c r="AM45" s="10"/>
       <c r="AN45" s="10"/>
       <c r="AO45" s="10"/>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP45" s="10"/>
+    </row>
+    <row r="46" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A46" s="10"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
       <c r="D46" s="10"/>
       <c r="E46" s="29"/>
-      <c r="F46" s="10"/>
+      <c r="F46" s="29"/>
       <c r="G46" s="10"/>
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
@@ -2788,14 +3047,15 @@
       <c r="AM46" s="10"/>
       <c r="AN46" s="10"/>
       <c r="AO46" s="10"/>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP46" s="10"/>
+    </row>
+    <row r="47" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A47" s="10"/>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
       <c r="D47" s="10"/>
       <c r="E47" s="29"/>
-      <c r="F47" s="10"/>
+      <c r="F47" s="29"/>
       <c r="G47" s="10"/>
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
@@ -2831,14 +3091,15 @@
       <c r="AM47" s="10"/>
       <c r="AN47" s="10"/>
       <c r="AO47" s="10"/>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP47" s="10"/>
+    </row>
+    <row r="48" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A48" s="10"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
       <c r="E48" s="29"/>
-      <c r="F48" s="10"/>
+      <c r="F48" s="29"/>
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
@@ -2874,14 +3135,15 @@
       <c r="AM48" s="10"/>
       <c r="AN48" s="10"/>
       <c r="AO48" s="10"/>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP48" s="10"/>
+    </row>
+    <row r="49" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A49" s="10"/>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
       <c r="D49" s="10"/>
       <c r="E49" s="29"/>
-      <c r="F49" s="10"/>
+      <c r="F49" s="29"/>
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
@@ -2917,14 +3179,15 @@
       <c r="AM49" s="10"/>
       <c r="AN49" s="10"/>
       <c r="AO49" s="10"/>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP49" s="10"/>
+    </row>
+    <row r="50" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A50" s="10"/>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
       <c r="E50" s="29"/>
-      <c r="F50" s="10"/>
+      <c r="F50" s="29"/>
       <c r="G50" s="10"/>
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
@@ -2960,14 +3223,15 @@
       <c r="AM50" s="10"/>
       <c r="AN50" s="10"/>
       <c r="AO50" s="10"/>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP50" s="10"/>
+    </row>
+    <row r="51" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A51" s="10"/>
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
       <c r="E51" s="29"/>
-      <c r="F51" s="10"/>
+      <c r="F51" s="29"/>
       <c r="G51" s="10"/>
       <c r="H51" s="10"/>
       <c r="I51" s="10"/>
@@ -3003,14 +3267,15 @@
       <c r="AM51" s="10"/>
       <c r="AN51" s="10"/>
       <c r="AO51" s="10"/>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP51" s="10"/>
+    </row>
+    <row r="52" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A52" s="10"/>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
       <c r="E52" s="29"/>
-      <c r="F52" s="10"/>
+      <c r="F52" s="29"/>
       <c r="G52" s="10"/>
       <c r="H52" s="10"/>
       <c r="I52" s="10"/>
@@ -3046,14 +3311,15 @@
       <c r="AM52" s="10"/>
       <c r="AN52" s="10"/>
       <c r="AO52" s="10"/>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP52" s="10"/>
+    </row>
+    <row r="53" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A53" s="10"/>
       <c r="B53" s="10"/>
       <c r="C53" s="10"/>
       <c r="D53" s="10"/>
       <c r="E53" s="29"/>
-      <c r="F53" s="10"/>
+      <c r="F53" s="29"/>
       <c r="G53" s="10"/>
       <c r="H53" s="10"/>
       <c r="I53" s="10"/>
@@ -3089,14 +3355,15 @@
       <c r="AM53" s="10"/>
       <c r="AN53" s="10"/>
       <c r="AO53" s="10"/>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP53" s="10"/>
+    </row>
+    <row r="54" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A54" s="10"/>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
       <c r="E54" s="29"/>
-      <c r="F54" s="10"/>
+      <c r="F54" s="29"/>
       <c r="G54" s="10"/>
       <c r="H54" s="10"/>
       <c r="I54" s="10"/>
@@ -3132,14 +3399,15 @@
       <c r="AM54" s="10"/>
       <c r="AN54" s="10"/>
       <c r="AO54" s="10"/>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP54" s="10"/>
+    </row>
+    <row r="55" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A55" s="10"/>
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
       <c r="E55" s="29"/>
-      <c r="F55" s="10"/>
+      <c r="F55" s="29"/>
       <c r="G55" s="10"/>
       <c r="H55" s="10"/>
       <c r="I55" s="10"/>
@@ -3175,14 +3443,15 @@
       <c r="AM55" s="10"/>
       <c r="AN55" s="10"/>
       <c r="AO55" s="10"/>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP55" s="10"/>
+    </row>
+    <row r="56" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A56" s="10"/>
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
       <c r="E56" s="29"/>
-      <c r="F56" s="10"/>
+      <c r="F56" s="29"/>
       <c r="G56" s="10"/>
       <c r="H56" s="10"/>
       <c r="I56" s="10"/>
@@ -3218,14 +3487,15 @@
       <c r="AM56" s="10"/>
       <c r="AN56" s="10"/>
       <c r="AO56" s="10"/>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP56" s="10"/>
+    </row>
+    <row r="57" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A57" s="10"/>
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
       <c r="E57" s="29"/>
-      <c r="F57" s="10"/>
+      <c r="F57" s="29"/>
       <c r="G57" s="10"/>
       <c r="H57" s="10"/>
       <c r="I57" s="10"/>
@@ -3261,14 +3531,15 @@
       <c r="AM57" s="10"/>
       <c r="AN57" s="10"/>
       <c r="AO57" s="10"/>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP57" s="10"/>
+    </row>
+    <row r="58" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A58" s="10"/>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
       <c r="E58" s="29"/>
-      <c r="F58" s="10"/>
+      <c r="F58" s="29"/>
       <c r="G58" s="10"/>
       <c r="H58" s="10"/>
       <c r="I58" s="10"/>
@@ -3304,14 +3575,15 @@
       <c r="AM58" s="10"/>
       <c r="AN58" s="10"/>
       <c r="AO58" s="10"/>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP58" s="10"/>
+    </row>
+    <row r="59" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A59" s="10"/>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
       <c r="E59" s="29"/>
-      <c r="F59" s="10"/>
+      <c r="F59" s="29"/>
       <c r="G59" s="10"/>
       <c r="H59" s="10"/>
       <c r="I59" s="10"/>
@@ -3347,14 +3619,15 @@
       <c r="AM59" s="10"/>
       <c r="AN59" s="10"/>
       <c r="AO59" s="10"/>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP59" s="10"/>
+    </row>
+    <row r="60" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A60" s="10"/>
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
       <c r="E60" s="29"/>
-      <c r="F60" s="10"/>
+      <c r="F60" s="29"/>
       <c r="G60" s="10"/>
       <c r="H60" s="10"/>
       <c r="I60" s="10"/>
@@ -3390,14 +3663,15 @@
       <c r="AM60" s="10"/>
       <c r="AN60" s="10"/>
       <c r="AO60" s="10"/>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP60" s="10"/>
+    </row>
+    <row r="61" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A61" s="10"/>
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
       <c r="E61" s="29"/>
-      <c r="F61" s="10"/>
+      <c r="F61" s="29"/>
       <c r="G61" s="10"/>
       <c r="H61" s="10"/>
       <c r="I61" s="10"/>
@@ -3433,14 +3707,15 @@
       <c r="AM61" s="10"/>
       <c r="AN61" s="10"/>
       <c r="AO61" s="10"/>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP61" s="10"/>
+    </row>
+    <row r="62" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A62" s="10"/>
       <c r="B62" s="10"/>
       <c r="C62" s="10"/>
       <c r="D62" s="10"/>
       <c r="E62" s="29"/>
-      <c r="F62" s="10"/>
+      <c r="F62" s="29"/>
       <c r="G62" s="10"/>
       <c r="H62" s="10"/>
       <c r="I62" s="10"/>
@@ -3476,14 +3751,15 @@
       <c r="AM62" s="10"/>
       <c r="AN62" s="10"/>
       <c r="AO62" s="10"/>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP62" s="10"/>
+    </row>
+    <row r="63" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A63" s="10"/>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
       <c r="E63" s="29"/>
-      <c r="F63" s="10"/>
+      <c r="F63" s="29"/>
       <c r="G63" s="10"/>
       <c r="H63" s="10"/>
       <c r="I63" s="10"/>
@@ -3519,14 +3795,15 @@
       <c r="AM63" s="10"/>
       <c r="AN63" s="10"/>
       <c r="AO63" s="10"/>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP63" s="10"/>
+    </row>
+    <row r="64" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A64" s="10"/>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
       <c r="D64" s="10"/>
       <c r="E64" s="29"/>
-      <c r="F64" s="10"/>
+      <c r="F64" s="29"/>
       <c r="G64" s="10"/>
       <c r="H64" s="10"/>
       <c r="I64" s="10"/>
@@ -3562,14 +3839,15 @@
       <c r="AM64" s="10"/>
       <c r="AN64" s="10"/>
       <c r="AO64" s="10"/>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP64" s="10"/>
+    </row>
+    <row r="65" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A65" s="10"/>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
       <c r="D65" s="10"/>
       <c r="E65" s="29"/>
-      <c r="F65" s="10"/>
+      <c r="F65" s="29"/>
       <c r="G65" s="10"/>
       <c r="H65" s="10"/>
       <c r="I65" s="10"/>
@@ -3605,14 +3883,15 @@
       <c r="AM65" s="10"/>
       <c r="AN65" s="10"/>
       <c r="AO65" s="10"/>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP65" s="10"/>
+    </row>
+    <row r="66" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A66" s="10"/>
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
       <c r="D66" s="10"/>
       <c r="E66" s="29"/>
-      <c r="F66" s="10"/>
+      <c r="F66" s="29"/>
       <c r="G66" s="10"/>
       <c r="H66" s="10"/>
       <c r="I66" s="10"/>
@@ -3648,14 +3927,15 @@
       <c r="AM66" s="10"/>
       <c r="AN66" s="10"/>
       <c r="AO66" s="10"/>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP66" s="10"/>
+    </row>
+    <row r="67" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A67" s="10"/>
       <c r="B67" s="10"/>
       <c r="C67" s="10"/>
       <c r="D67" s="10"/>
       <c r="E67" s="29"/>
-      <c r="F67" s="10"/>
+      <c r="F67" s="29"/>
       <c r="G67" s="10"/>
       <c r="H67" s="10"/>
       <c r="I67" s="10"/>
@@ -3691,14 +3971,15 @@
       <c r="AM67" s="10"/>
       <c r="AN67" s="10"/>
       <c r="AO67" s="10"/>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP67" s="10"/>
+    </row>
+    <row r="68" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A68" s="10"/>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
       <c r="D68" s="10"/>
       <c r="E68" s="29"/>
-      <c r="F68" s="10"/>
+      <c r="F68" s="29"/>
       <c r="G68" s="10"/>
       <c r="H68" s="10"/>
       <c r="I68" s="10"/>
@@ -3734,14 +4015,15 @@
       <c r="AM68" s="10"/>
       <c r="AN68" s="10"/>
       <c r="AO68" s="10"/>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP68" s="10"/>
+    </row>
+    <row r="69" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A69" s="10"/>
       <c r="B69" s="10"/>
       <c r="C69" s="10"/>
       <c r="D69" s="10"/>
       <c r="E69" s="29"/>
-      <c r="F69" s="10"/>
+      <c r="F69" s="29"/>
       <c r="G69" s="10"/>
       <c r="H69" s="10"/>
       <c r="I69" s="10"/>
@@ -3777,14 +4059,15 @@
       <c r="AM69" s="10"/>
       <c r="AN69" s="10"/>
       <c r="AO69" s="10"/>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP69" s="10"/>
+    </row>
+    <row r="70" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A70" s="10"/>
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
       <c r="D70" s="10"/>
       <c r="E70" s="29"/>
-      <c r="F70" s="10"/>
+      <c r="F70" s="29"/>
       <c r="G70" s="10"/>
       <c r="H70" s="10"/>
       <c r="I70" s="10"/>
@@ -3820,14 +4103,15 @@
       <c r="AM70" s="10"/>
       <c r="AN70" s="10"/>
       <c r="AO70" s="10"/>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP70" s="10"/>
+    </row>
+    <row r="71" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A71" s="10"/>
       <c r="B71" s="10"/>
       <c r="C71" s="10"/>
       <c r="D71" s="10"/>
       <c r="E71" s="29"/>
-      <c r="F71" s="10"/>
+      <c r="F71" s="29"/>
       <c r="G71" s="10"/>
       <c r="H71" s="10"/>
       <c r="I71" s="10"/>
@@ -3863,14 +4147,15 @@
       <c r="AM71" s="10"/>
       <c r="AN71" s="10"/>
       <c r="AO71" s="10"/>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP71" s="10"/>
+    </row>
+    <row r="72" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A72" s="10"/>
       <c r="B72" s="10"/>
       <c r="C72" s="10"/>
       <c r="D72" s="10"/>
       <c r="E72" s="29"/>
-      <c r="F72" s="10"/>
+      <c r="F72" s="29"/>
       <c r="G72" s="10"/>
       <c r="H72" s="10"/>
       <c r="I72" s="10"/>
@@ -3906,14 +4191,15 @@
       <c r="AM72" s="10"/>
       <c r="AN72" s="10"/>
       <c r="AO72" s="10"/>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP72" s="10"/>
+    </row>
+    <row r="73" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A73" s="10"/>
       <c r="B73" s="10"/>
       <c r="C73" s="10"/>
       <c r="D73" s="10"/>
       <c r="E73" s="29"/>
-      <c r="F73" s="10"/>
+      <c r="F73" s="29"/>
       <c r="G73" s="10"/>
       <c r="H73" s="10"/>
       <c r="I73" s="10"/>
@@ -3949,14 +4235,15 @@
       <c r="AM73" s="10"/>
       <c r="AN73" s="10"/>
       <c r="AO73" s="10"/>
-    </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP73" s="10"/>
+    </row>
+    <row r="74" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A74" s="10"/>
       <c r="B74" s="10"/>
       <c r="C74" s="10"/>
       <c r="D74" s="10"/>
       <c r="E74" s="29"/>
-      <c r="F74" s="10"/>
+      <c r="F74" s="29"/>
       <c r="G74" s="10"/>
       <c r="H74" s="10"/>
       <c r="I74" s="10"/>
@@ -3992,14 +4279,15 @@
       <c r="AM74" s="10"/>
       <c r="AN74" s="10"/>
       <c r="AO74" s="10"/>
-    </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP74" s="10"/>
+    </row>
+    <row r="75" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A75" s="10"/>
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
       <c r="D75" s="10"/>
       <c r="E75" s="29"/>
-      <c r="F75" s="10"/>
+      <c r="F75" s="29"/>
       <c r="G75" s="10"/>
       <c r="H75" s="10"/>
       <c r="I75" s="10"/>
@@ -4035,14 +4323,15 @@
       <c r="AM75" s="10"/>
       <c r="AN75" s="10"/>
       <c r="AO75" s="10"/>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP75" s="10"/>
+    </row>
+    <row r="76" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A76" s="10"/>
       <c r="B76" s="10"/>
       <c r="C76" s="10"/>
       <c r="D76" s="10"/>
       <c r="E76" s="29"/>
-      <c r="F76" s="10"/>
+      <c r="F76" s="29"/>
       <c r="G76" s="10"/>
       <c r="H76" s="10"/>
       <c r="I76" s="10"/>
@@ -4078,14 +4367,15 @@
       <c r="AM76" s="10"/>
       <c r="AN76" s="10"/>
       <c r="AO76" s="10"/>
-    </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP76" s="10"/>
+    </row>
+    <row r="77" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A77" s="10"/>
       <c r="B77" s="10"/>
       <c r="C77" s="10"/>
       <c r="D77" s="10"/>
       <c r="E77" s="29"/>
-      <c r="F77" s="10"/>
+      <c r="F77" s="29"/>
       <c r="G77" s="10"/>
       <c r="H77" s="10"/>
       <c r="I77" s="10"/>
@@ -4121,14 +4411,15 @@
       <c r="AM77" s="10"/>
       <c r="AN77" s="10"/>
       <c r="AO77" s="10"/>
-    </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP77" s="10"/>
+    </row>
+    <row r="78" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A78" s="10"/>
       <c r="B78" s="10"/>
       <c r="C78" s="10"/>
       <c r="D78" s="10"/>
       <c r="E78" s="29"/>
-      <c r="F78" s="10"/>
+      <c r="F78" s="29"/>
       <c r="G78" s="10"/>
       <c r="H78" s="10"/>
       <c r="I78" s="10"/>
@@ -4164,14 +4455,15 @@
       <c r="AM78" s="10"/>
       <c r="AN78" s="10"/>
       <c r="AO78" s="10"/>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP78" s="10"/>
+    </row>
+    <row r="79" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A79" s="10"/>
       <c r="B79" s="10"/>
       <c r="C79" s="10"/>
       <c r="D79" s="10"/>
       <c r="E79" s="29"/>
-      <c r="F79" s="10"/>
+      <c r="F79" s="29"/>
       <c r="G79" s="10"/>
       <c r="H79" s="10"/>
       <c r="I79" s="10"/>
@@ -4207,14 +4499,15 @@
       <c r="AM79" s="10"/>
       <c r="AN79" s="10"/>
       <c r="AO79" s="10"/>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP79" s="10"/>
+    </row>
+    <row r="80" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A80" s="10"/>
       <c r="B80" s="10"/>
       <c r="C80" s="10"/>
       <c r="D80" s="10"/>
       <c r="E80" s="29"/>
-      <c r="F80" s="10"/>
+      <c r="F80" s="29"/>
       <c r="G80" s="10"/>
       <c r="H80" s="10"/>
       <c r="I80" s="10"/>
@@ -4250,14 +4543,15 @@
       <c r="AM80" s="10"/>
       <c r="AN80" s="10"/>
       <c r="AO80" s="10"/>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP80" s="10"/>
+    </row>
+    <row r="81" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A81" s="10"/>
       <c r="B81" s="10"/>
       <c r="C81" s="10"/>
       <c r="D81" s="10"/>
       <c r="E81" s="29"/>
-      <c r="F81" s="10"/>
+      <c r="F81" s="29"/>
       <c r="G81" s="10"/>
       <c r="H81" s="10"/>
       <c r="I81" s="10"/>
@@ -4293,14 +4587,15 @@
       <c r="AM81" s="10"/>
       <c r="AN81" s="10"/>
       <c r="AO81" s="10"/>
-    </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP81" s="10"/>
+    </row>
+    <row r="82" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A82" s="10"/>
       <c r="B82" s="10"/>
       <c r="C82" s="10"/>
       <c r="D82" s="10"/>
       <c r="E82" s="29"/>
-      <c r="F82" s="10"/>
+      <c r="F82" s="29"/>
       <c r="G82" s="10"/>
       <c r="H82" s="10"/>
       <c r="I82" s="10"/>
@@ -4336,14 +4631,15 @@
       <c r="AM82" s="10"/>
       <c r="AN82" s="10"/>
       <c r="AO82" s="10"/>
-    </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP82" s="10"/>
+    </row>
+    <row r="83" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A83" s="10"/>
       <c r="B83" s="10"/>
       <c r="C83" s="10"/>
       <c r="D83" s="10"/>
       <c r="E83" s="29"/>
-      <c r="F83" s="10"/>
+      <c r="F83" s="29"/>
       <c r="G83" s="10"/>
       <c r="H83" s="10"/>
       <c r="I83" s="10"/>
@@ -4379,14 +4675,15 @@
       <c r="AM83" s="10"/>
       <c r="AN83" s="10"/>
       <c r="AO83" s="10"/>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP83" s="10"/>
+    </row>
+    <row r="84" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A84" s="10"/>
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
       <c r="D84" s="10"/>
       <c r="E84" s="29"/>
-      <c r="F84" s="10"/>
+      <c r="F84" s="29"/>
       <c r="G84" s="10"/>
       <c r="H84" s="10"/>
       <c r="I84" s="10"/>
@@ -4422,14 +4719,15 @@
       <c r="AM84" s="10"/>
       <c r="AN84" s="10"/>
       <c r="AO84" s="10"/>
-    </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP84" s="10"/>
+    </row>
+    <row r="85" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A85" s="10"/>
       <c r="B85" s="10"/>
       <c r="C85" s="10"/>
       <c r="D85" s="10"/>
       <c r="E85" s="29"/>
-      <c r="F85" s="10"/>
+      <c r="F85" s="29"/>
       <c r="G85" s="10"/>
       <c r="H85" s="10"/>
       <c r="I85" s="10"/>
@@ -4465,14 +4763,15 @@
       <c r="AM85" s="10"/>
       <c r="AN85" s="10"/>
       <c r="AO85" s="10"/>
-    </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP85" s="10"/>
+    </row>
+    <row r="86" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A86" s="10"/>
       <c r="B86" s="10"/>
       <c r="C86" s="10"/>
       <c r="D86" s="10"/>
       <c r="E86" s="29"/>
-      <c r="F86" s="10"/>
+      <c r="F86" s="29"/>
       <c r="G86" s="10"/>
       <c r="H86" s="10"/>
       <c r="I86" s="10"/>
@@ -4508,14 +4807,15 @@
       <c r="AM86" s="10"/>
       <c r="AN86" s="10"/>
       <c r="AO86" s="10"/>
-    </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP86" s="10"/>
+    </row>
+    <row r="87" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A87" s="10"/>
       <c r="B87" s="10"/>
       <c r="C87" s="10"/>
       <c r="D87" s="10"/>
       <c r="E87" s="29"/>
-      <c r="F87" s="10"/>
+      <c r="F87" s="29"/>
       <c r="G87" s="10"/>
       <c r="H87" s="10"/>
       <c r="I87" s="10"/>
@@ -4551,14 +4851,15 @@
       <c r="AM87" s="10"/>
       <c r="AN87" s="10"/>
       <c r="AO87" s="10"/>
-    </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP87" s="10"/>
+    </row>
+    <row r="88" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A88" s="10"/>
       <c r="B88" s="10"/>
       <c r="C88" s="10"/>
       <c r="D88" s="10"/>
       <c r="E88" s="29"/>
-      <c r="F88" s="10"/>
+      <c r="F88" s="29"/>
       <c r="G88" s="10"/>
       <c r="H88" s="10"/>
       <c r="I88" s="10"/>
@@ -4594,14 +4895,15 @@
       <c r="AM88" s="10"/>
       <c r="AN88" s="10"/>
       <c r="AO88" s="10"/>
-    </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP88" s="10"/>
+    </row>
+    <row r="89" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A89" s="10"/>
       <c r="B89" s="10"/>
       <c r="C89" s="10"/>
       <c r="D89" s="10"/>
       <c r="E89" s="29"/>
-      <c r="F89" s="10"/>
+      <c r="F89" s="29"/>
       <c r="G89" s="10"/>
       <c r="H89" s="10"/>
       <c r="I89" s="10"/>
@@ -4637,14 +4939,15 @@
       <c r="AM89" s="10"/>
       <c r="AN89" s="10"/>
       <c r="AO89" s="10"/>
-    </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP89" s="10"/>
+    </row>
+    <row r="90" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A90" s="10"/>
       <c r="B90" s="10"/>
       <c r="C90" s="10"/>
       <c r="D90" s="10"/>
       <c r="E90" s="29"/>
-      <c r="F90" s="10"/>
+      <c r="F90" s="29"/>
       <c r="G90" s="10"/>
       <c r="H90" s="10"/>
       <c r="I90" s="10"/>
@@ -4680,14 +4983,15 @@
       <c r="AM90" s="10"/>
       <c r="AN90" s="10"/>
       <c r="AO90" s="10"/>
-    </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP90" s="10"/>
+    </row>
+    <row r="91" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A91" s="10"/>
       <c r="B91" s="10"/>
       <c r="C91" s="10"/>
       <c r="D91" s="10"/>
       <c r="E91" s="29"/>
-      <c r="F91" s="10"/>
+      <c r="F91" s="29"/>
       <c r="G91" s="10"/>
       <c r="H91" s="10"/>
       <c r="I91" s="10"/>
@@ -4723,14 +5027,15 @@
       <c r="AM91" s="10"/>
       <c r="AN91" s="10"/>
       <c r="AO91" s="10"/>
-    </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP91" s="10"/>
+    </row>
+    <row r="92" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A92" s="10"/>
       <c r="B92" s="10"/>
       <c r="C92" s="10"/>
       <c r="D92" s="10"/>
       <c r="E92" s="29"/>
-      <c r="F92" s="10"/>
+      <c r="F92" s="29"/>
       <c r="G92" s="10"/>
       <c r="H92" s="10"/>
       <c r="I92" s="10"/>
@@ -4766,14 +5071,15 @@
       <c r="AM92" s="10"/>
       <c r="AN92" s="10"/>
       <c r="AO92" s="10"/>
-    </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP92" s="10"/>
+    </row>
+    <row r="93" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A93" s="10"/>
       <c r="B93" s="10"/>
       <c r="C93" s="10"/>
       <c r="D93" s="10"/>
       <c r="E93" s="29"/>
-      <c r="F93" s="10"/>
+      <c r="F93" s="29"/>
       <c r="G93" s="10"/>
       <c r="H93" s="10"/>
       <c r="I93" s="10"/>
@@ -4809,14 +5115,15 @@
       <c r="AM93" s="10"/>
       <c r="AN93" s="10"/>
       <c r="AO93" s="10"/>
-    </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP93" s="10"/>
+    </row>
+    <row r="94" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A94" s="10"/>
       <c r="B94" s="10"/>
       <c r="C94" s="10"/>
       <c r="D94" s="10"/>
       <c r="E94" s="29"/>
-      <c r="F94" s="10"/>
+      <c r="F94" s="29"/>
       <c r="G94" s="10"/>
       <c r="H94" s="10"/>
       <c r="I94" s="10"/>
@@ -4852,14 +5159,15 @@
       <c r="AM94" s="10"/>
       <c r="AN94" s="10"/>
       <c r="AO94" s="10"/>
-    </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP94" s="10"/>
+    </row>
+    <row r="95" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A95" s="10"/>
       <c r="B95" s="10"/>
       <c r="C95" s="10"/>
       <c r="D95" s="10"/>
       <c r="E95" s="29"/>
-      <c r="F95" s="10"/>
+      <c r="F95" s="29"/>
       <c r="G95" s="10"/>
       <c r="H95" s="10"/>
       <c r="I95" s="10"/>
@@ -4895,78 +5203,70 @@
       <c r="AM95" s="10"/>
       <c r="AN95" s="10"/>
       <c r="AO95" s="10"/>
-    </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP95" s="10"/>
+    </row>
+    <row r="96" spans="1:42" x14ac:dyDescent="0.2">
       <c r="C96" s="10"/>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C97" s="10"/>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C98" s="10"/>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C99" s="10"/>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C100" s="10"/>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C101" s="10"/>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C102" s="10"/>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C103" s="10"/>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C104" s="10"/>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C105" s="10"/>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C106" s="10"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMH100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="24.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="982" style="0" width="9.17"/>
+    <col min="1" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28.5" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
+    <col min="982" max="1023" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:1022" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
         <v>87</v>
       </c>
@@ -4974,8 +5274,9 @@
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
-    </row>
-    <row r="4" s="31" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:1022" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
         <v>15</v>
       </c>
@@ -4990,510 +5291,512 @@
       </c>
       <c r="E4" s="31" t="s">
         <v>91</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>103</v>
       </c>
       <c r="AMF4" s="32"/>
       <c r="AMG4" s="32"/>
       <c r="AMH4" s="32"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5">
         <v>5</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A6" s="10"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A10" s="10"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A12" s="10"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="10"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="10"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="10"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="10"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="10"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="10"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="10"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="10"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="10"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="10"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="10"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="10"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="10"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="10"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="10"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="10"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="10"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="10"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="10"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="10"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="10"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="10"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="10"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="10"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="10"/>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="10"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="10"/>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="10"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="10"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="10"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="10"/>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="10"/>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="10"/>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="10"/>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="10"/>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="10"/>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="10"/>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="10"/>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="10"/>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" s="10"/>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="10"/>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="10"/>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="10"/>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="10"/>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="10"/>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="10"/>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="10"/>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="10"/>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" s="10"/>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" s="10"/>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="10"/>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" s="10"/>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" s="10"/>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" s="10"/>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="10"/>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="10"/>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="10"/>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" s="10"/>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" s="10"/>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" s="10"/>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" s="10"/>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" s="10"/>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" s="10"/>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" s="10"/>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" s="10"/>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" s="10"/>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" s="10"/>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" s="10"/>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" s="10"/>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" s="10"/>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" s="10"/>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" s="10"/>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" s="10"/>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" s="10"/>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" s="10"/>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" s="10"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A5:A100" type="list">
-      <formula1>Experiments!$A$11:$A$110</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+          <x14:formula1>
+            <xm:f>Experiments!$A$11:$A$110</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>A5:A100</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="71.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="70.34"/>
+    <col min="1" max="1" width="42" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+    <col min="4" max="4" width="71.1640625" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="7" max="7" width="70.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>95</v>
       </c>
       <c r="D1" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
       <c r="G1" s="33" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" t="s">
         <v>103</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>107</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>107</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>108</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" t="s">
         <v>103</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>103</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F10" s="0" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F11" s="0" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F12" s="0" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
         <v>103</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Sample Name to the prefill of all  the templates
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Experiment_Infinium_24_v3_5_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Experiment_Infinium_24_v3_5_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/tests/valid_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14446785-5EE6-3846-82F5-77ACB8D89B72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DED4F94-8171-114D-B386-D91A0824732F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16360" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
@@ -163,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="111">
   <si>
     <t>Experiment Submission Template</t>
   </si>
@@ -493,6 +493,9 @@
   </si>
   <si>
     <t>Test comment</t>
+  </si>
+  <si>
+    <t>Source Sample Name</t>
   </si>
 </sst>
 </file>
@@ -5247,26 +5250,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMH100"/>
+  <dimension ref="A1:AMI100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="24.33203125" customWidth="1"/>
-    <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" customWidth="1"/>
-    <col min="5" max="5" width="28.5" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" customWidth="1"/>
-    <col min="982" max="1023" width="9.1640625" customWidth="1"/>
+    <col min="1" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="6" max="6" width="28.5" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="983" max="1024" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1022" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1023" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
         <v>87</v>
       </c>
@@ -5275,127 +5278,131 @@
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-    </row>
-    <row r="4" spans="1:1022" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:1023" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="D4" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="E4" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="F4" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="G4" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="AMF4" s="32"/>
       <c r="AMG4" s="32"/>
       <c r="AMH4" s="32"/>
-    </row>
-    <row r="5" spans="1:1022" x14ac:dyDescent="0.2">
+      <c r="AMI4" s="32"/>
+    </row>
+    <row r="5" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>92</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>93</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A6" s="10"/>
     </row>
-    <row r="7" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
     </row>
-    <row r="8" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
     </row>
-    <row r="9" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
     </row>
-    <row r="10" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A10" s="10"/>
     </row>
-    <row r="11" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
     </row>
-    <row r="12" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A12" s="10"/>
     </row>
-    <row r="13" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
     </row>
-    <row r="14" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
     </row>
-    <row r="15" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
     </row>
-    <row r="16" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="10"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
-      <c r="C19" s="8"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="10"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="10"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="10"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="10"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="10"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="10"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="10"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>